<commit_message>
first test of new testheirarchies
</commit_message>
<xml_diff>
--- a/categorySort/notebooks/data/completedHierarchy.xlsx
+++ b/categorySort/notebooks/data/completedHierarchy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfad3d3100e0b584/addedIQ/Random/categorySort/notebooks/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jh\Desktop\Projects\Random\categorySort\notebooks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{DCBF2EFE-023C-4809-953F-599DC033B47A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7F59AC54-6480-43C7-BE10-8572587CA753}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD8A1F2-0E47-45C7-864F-F569223749C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3893" yWindow="83" windowWidth="18225" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12254" uniqueCount="5322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12253" uniqueCount="5322">
   <si>
     <t>Survey</t>
   </si>
@@ -16428,8 +16428,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K5050"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D239" sqref="D239"/>
+    <sheetView tabSelected="1" topLeftCell="A213" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C240" sqref="C240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -19128,10 +19128,7 @@
         <v>2</v>
       </c>
       <c r="C239" t="s">
-        <v>5057</v>
-      </c>
-      <c r="D239" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
got the category assignments, cant seem to get it into excel sheet (TestHierarchies.py)
</commit_message>
<xml_diff>
--- a/categorySort/notebooks/data/completedHierarchy.xlsx
+++ b/categorySort/notebooks/data/completedHierarchy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jh\Desktop\Projects\Random\categorySort\notebooks\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mh\OneDrive\addedIQ\Random\categorySort\notebooks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD8A1F2-0E47-45C7-864F-F569223749C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CD409F-33B0-41D0-9CE1-49FC34E6AE57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3893" yWindow="83" windowWidth="18225" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16428,8 +16428,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K5050"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A213" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C240" sqref="C240"/>
+    <sheetView tabSelected="1" topLeftCell="A2123" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2186" sqref="C2186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>